<commit_message>
2nd testing of object detection using YOLOv8 with 817 data
</commit_message>
<xml_diff>
--- a/result/result training.xlsx
+++ b/result/result training.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\number-plate-recognition\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D98932C-5D34-4754-8071-F29305D0E15B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AEC597-1F11-4A58-9540-D8D62ED8022E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22992" yWindow="384" windowWidth="21600" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing" sheetId="3" r:id="rId1"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>Jumlah</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Train</t>
   </si>
@@ -39,15 +36,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Jumlah Dataset</t>
-  </si>
-  <si>
-    <t>Percobaan</t>
-  </si>
-  <si>
-    <t>Akurasi</t>
-  </si>
-  <si>
     <t>Epoch</t>
   </si>
   <si>
@@ -70,12 +58,33 @@
   </si>
   <si>
     <t>Confussion Matrix Testing</t>
+  </si>
+  <si>
+    <t>Result Saved</t>
+  </si>
+  <si>
+    <t>runs\detect\train19\weights</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total Dataset</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -180,21 +189,21 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -203,22 +212,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -436,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BF86F8-5004-4712-B9DC-99E03C733B38}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -451,83 +469,93 @@
     <col min="7" max="7" width="11.28515625" style="1" customWidth="1"/>
     <col min="8" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="11" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="14" width="14.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8" t="s">
+      <c r="J2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="10"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>440</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.9</v>
       </c>
       <c r="D3" s="3">
-        <f>ROUNDUP(C3*B3,2)</f>
+        <f>ROUNDUP(C3*B3,0)</f>
         <v>396</v>
       </c>
       <c r="E3" s="3">
@@ -553,49 +581,115 @@
         <v>0</v>
       </c>
       <c r="L3" s="3">
+        <f>H3+I3+J3+K3</f>
+        <v>44</v>
+      </c>
+      <c r="M3" s="3">
         <f>((H3+I3)/(H3+I3+J3+K3))*100</f>
         <v>0</v>
       </c>
-      <c r="M3" s="3" t="e">
+      <c r="N3" s="3" t="e">
         <f>(H3/(H3+I3))*100</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>817</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D4" s="3">
+        <f>ROUNDUP(C4*B4,0)</f>
+        <v>736</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:F5" si="0">B4-D4</f>
+        <v>81</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3">
+        <v>45</v>
+      </c>
+      <c r="I4" s="3">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3">
+        <v>36</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L5" si="1">H4+I4+J4+K4</f>
+        <v>101</v>
+      </c>
+      <c r="M4" s="11">
+        <f>((H4+I4)/(H4+I4+J4+K4))*100</f>
+        <v>64.356435643564353</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" ref="N4:N5" si="2">(H4/(H4+I4))*100</f>
+        <v>69.230769230769226</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D5" s="3">
+        <f>ROUNDUP(C5*B5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="L5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="3" t="e">
+        <f>((H5+I5)/(H5+I5+J5+K5))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N5" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O5" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="L1:L2"/>
+  <mergeCells count="9">
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="E1:F1"/>

</xml_diff>

<commit_message>
3rd testing of object detection using 817 data & 10 epoch
</commit_message>
<xml_diff>
--- a/result/result training.xlsx
+++ b/result/result training.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\number-plate-recognition\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AEC597-1F11-4A58-9540-D8D62ED8022E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF5C0B0-313F-4A32-A28D-691969CE3553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22992" yWindow="384" windowWidth="21600" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="21600" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Train</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Result Saved</t>
   </si>
   <si>
-    <t>runs\detect\train19\weights</t>
-  </si>
-  <si>
     <t>Accuracy</t>
   </si>
   <si>
@@ -76,6 +73,21 @@
   </si>
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>runs\detect\train202</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>runs\detect\train192</t>
+  </si>
+  <si>
+    <t>runs\detect\train20</t>
+  </si>
+  <si>
+    <t>runs\detect\train19</t>
   </si>
 </sst>
 </file>
@@ -83,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -203,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -215,29 +227,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BF86F8-5004-4712-B9DC-99E03C733B38}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -470,61 +485,62 @@
     <col min="8" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="11" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="29.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="16" width="21.7109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="7" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="P1" s="6"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="G2" s="9"/>
       <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
@@ -538,13 +554,18 @@
         <v>6</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="M2" s="9"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -593,8 +614,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -634,59 +656,148 @@
         <f t="shared" ref="L4:L5" si="1">H4+I4+J4+K4</f>
         <v>101</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="5">
         <f>((H4+I4)/(H4+I4+J4+K4))*100</f>
         <v>64.356435643564353</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="5">
         <f t="shared" ref="N4:N5" si="2">(H4/(H4+I4))*100</f>
         <v>69.230769230769226</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <v>817</v>
+      </c>
       <c r="C5" s="3">
         <v>0.9</v>
       </c>
       <c r="D5" s="3">
         <f>ROUNDUP(C5*B5,0)</f>
-        <v>0</v>
+        <v>736</v>
       </c>
       <c r="E5" s="3">
         <v>0.1</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3">
+        <v>77</v>
+      </c>
+      <c r="I5" s="3">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3">
+        <v>4</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
       <c r="L5" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="3" t="e">
+        <v>91</v>
+      </c>
+      <c r="M5" s="5">
         <f>((H5+I5)/(H5+I5+J5+K5))*100</f>
+        <v>95.604395604395606</v>
+      </c>
+      <c r="N5" s="5">
+        <f t="shared" si="2"/>
+        <v>88.505747126436788</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <f t="shared" ref="D6:D7" si="3">ROUNDUP(C6*B6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <f t="shared" ref="F6:F7" si="4">B6-D6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3">
+        <f t="shared" ref="L6:L7" si="5">H6+I6+J6+K6</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="3" t="e">
+        <f t="shared" ref="M6:M7" si="6">((H6+I6)/(H6+I6+J6+K6))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N5" s="3" t="e">
-        <f t="shared" si="2"/>
+      <c r="N6" s="3" t="e">
+        <f t="shared" ref="N6:N7" si="7">(H6/(H6+I6))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O5" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="3" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" s="3" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="O1:O2"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
@@ -695,6 +806,7 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
4th testing of OB using 1419 data, 5 epoch, and do the spliting data to data train, val, test
</commit_message>
<xml_diff>
--- a/result/result training.xlsx
+++ b/result/result training.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\number-plate-recognition\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF5C0B0-313F-4A32-A28D-691969CE3553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5CA58D-69AF-46D9-A481-20B740552B9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="384" windowWidth="21600" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Testing" sheetId="3" r:id="rId1"/>
+    <sheet name="Real" sheetId="3" r:id="rId1"/>
+    <sheet name="Modif" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
   <si>
     <t>Train</t>
   </si>
@@ -88,6 +89,18 @@
   </si>
   <si>
     <t>runs\detect\train19</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>runs\detect\train21</t>
+  </si>
+  <si>
+    <t>runs\detect\train212</t>
   </si>
 </sst>
 </file>
@@ -215,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -231,7 +244,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,7 +271,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,103 +494,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BF86F8-5004-4712-B9DC-99E03C733B38}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" customWidth="1"/>
-    <col min="8" max="12" width="9.140625" style="1"/>
-    <col min="13" max="13" width="11" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="21.7109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="1" customWidth="1"/>
+    <col min="10" max="14" width="9.109375" style="1"/>
+    <col min="15" max="15" width="11" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" style="1" customWidth="1"/>
+    <col min="17" max="18" width="21.6640625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="8" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="P1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
+      <c r="R1" s="15"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="11"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="11"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -583,40 +620,47 @@
         <v>0.1</v>
       </c>
       <c r="F3" s="3">
-        <f>B3-D3</f>
+        <f>ROUNDDOWN(E3*B3,0)</f>
         <v>44</v>
       </c>
       <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <f>G3*B3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
         <v>5</v>
       </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0</v>
-      </c>
       <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
         <v>44</v>
       </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <f>H3+I3+J3+K3</f>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <f>J3+K3+L3+M3</f>
         <v>44</v>
       </c>
-      <c r="M3" s="3">
-        <f>((H3+I3)/(H3+I3+J3+K3))*100</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="3" t="e">
-        <f>(H3/(H3+I3))*100</f>
+      <c r="O3" s="3">
+        <f>((J3+K3)/(J3+K3+L3+M3))*100</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="e">
+        <f>(J3/(J3+K3))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -634,44 +678,51 @@
         <v>0.1</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F5" si="0">B4-D4</f>
+        <f>ROUNDDOWN(E4*B4,0)</f>
         <v>81</v>
       </c>
       <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" ref="H4:H7" si="0">G4*B4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
         <v>5</v>
       </c>
-      <c r="H4" s="3">
+      <c r="J4" s="3">
         <v>45</v>
       </c>
-      <c r="I4" s="3">
+      <c r="K4" s="3">
         <v>20</v>
       </c>
-      <c r="J4" s="3">
+      <c r="L4" s="3">
         <v>36</v>
       </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" ref="L4:L5" si="1">H4+I4+J4+K4</f>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" ref="N4:N5" si="1">J4+K4+L4+M4</f>
         <v>101</v>
       </c>
-      <c r="M4" s="5">
-        <f>((H4+I4)/(H4+I4+J4+K4))*100</f>
+      <c r="O4" s="5">
+        <f>((J4+K4)/(J4+K4+L4+M4))*100</f>
         <v>64.356435643564353</v>
       </c>
-      <c r="N4" s="5">
-        <f t="shared" ref="N4:N5" si="2">(H4/(H4+I4))*100</f>
+      <c r="P4" s="5">
+        <f t="shared" ref="P4:P5" si="2">(J4/(J4+K4))*100</f>
         <v>69.230769230769226</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -689,56 +740,470 @@
         <v>0.1</v>
       </c>
       <c r="F5" s="3">
+        <f>ROUNDDOWN(E5*B5,0)</f>
+        <v>81</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
-        <v>81</v>
-      </c>
-      <c r="G5" s="3">
-        <v>10</v>
-      </c>
-      <c r="H5" s="3">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="I5" s="3">
         <v>10</v>
       </c>
       <c r="J5" s="3">
+        <v>77</v>
+      </c>
+      <c r="K5" s="3">
+        <v>10</v>
+      </c>
+      <c r="L5" s="3">
         <v>4</v>
       </c>
-      <c r="K5" s="3">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="M5" s="5">
-        <f>((H5+I5)/(H5+I5+J5+K5))*100</f>
+      <c r="O5" s="5">
+        <f>((J5+K5)/(J5+K5+L5+M5))*100</f>
         <v>95.604395604395606</v>
       </c>
-      <c r="N5" s="5">
+      <c r="P5" s="5">
         <f t="shared" si="2"/>
         <v>88.505747126436788</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1419</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="3">
+        <f>ROUND(C6*B6,0)</f>
+        <v>1135</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="3">
+        <f>ROUND(E6*B6,0)</f>
+        <v>142</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="3">
+        <f>ROUND(G6*B6,0)</f>
+        <v>142</v>
+      </c>
+      <c r="I6" s="3">
+        <v>5</v>
+      </c>
+      <c r="J6" s="3">
+        <v>120</v>
+      </c>
+      <c r="K6" s="3">
+        <v>24</v>
+      </c>
+      <c r="L6" s="3">
+        <v>22</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" ref="N6:N7" si="3">J6+K6+L6+M6</f>
+        <v>166</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" ref="O6:O7" si="4">((J6+K6)/(J6+K6+L6+M6))*100</f>
+        <v>86.746987951807228</v>
+      </c>
+      <c r="P6" s="5">
+        <f t="shared" ref="P6:P7" si="5">(J6/(J6+K6))*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <f>ROUND(C7*B7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <f>ROUND(E7*B7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
+        <f>ROUND(G7*B7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="I1:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5ED25B5-2FA0-42FF-A500-B0ACF9209455}">
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="1" customWidth="1"/>
+    <col min="10" max="14" width="9.109375" style="1"/>
+    <col min="15" max="15" width="11" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" style="1" customWidth="1"/>
+    <col min="17" max="18" width="21.6640625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="15"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>440</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D3" s="3">
+        <f>ROUNDUP(C3*B3,0)</f>
+        <v>396</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="3">
+        <f>B3-D3</f>
+        <v>44</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>44</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <f>J3+K3+L3+M3</f>
+        <v>44</v>
+      </c>
+      <c r="O3" s="3">
+        <f>((J3+K3)/(J3+K3+L3+M3))*100</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="3" t="e">
+        <f>(J3/(J3+K3))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>920</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="D4" s="3">
+        <f>ROUNDUP(C4*B4,0)</f>
+        <v>736</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>92</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>92</v>
+      </c>
+      <c r="I4" s="3">
+        <v>5</v>
+      </c>
+      <c r="J4" s="3">
+        <v>45</v>
+      </c>
+      <c r="K4" s="3">
+        <v>20</v>
+      </c>
+      <c r="L4" s="3">
+        <v>36</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" ref="N4:N7" si="0">J4+K4+L4+M4</f>
+        <v>101</v>
+      </c>
+      <c r="O4" s="5">
+        <f>((J4+K4)/(J4+K4+L4+M4))*100</f>
+        <v>64.356435643564353</v>
+      </c>
+      <c r="P4" s="5">
+        <f t="shared" ref="P4:P7" si="1">(J4/(J4+K4))*100</f>
+        <v>69.230769230769226</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>920</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="D5" s="3">
+        <f>ROUNDUP(C5*B5,0)</f>
+        <v>736</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>92</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>92</v>
+      </c>
+      <c r="I5" s="3">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3">
+        <v>77</v>
+      </c>
+      <c r="K5" s="3">
+        <v>10</v>
+      </c>
+      <c r="L5" s="3">
+        <v>4</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="O5" s="5">
+        <f>((J5+K5)/(J5+K5+L5+M5))*100</f>
+        <v>95.604395604395606</v>
+      </c>
+      <c r="P5" s="5">
+        <f t="shared" si="1"/>
+        <v>88.505747126436788</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3">
-        <f t="shared" ref="D6:D7" si="3">ROUNDUP(C6*B6,0)</f>
+        <f t="shared" ref="D6:D7" si="2">ROUNDUP(C6*B6,0)</f>
         <v>0</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3">
-        <f t="shared" ref="F6:F7" si="4">B6-D6</f>
+        <f t="shared" ref="F4:F7" si="3">B6-D6</f>
         <v>0</v>
       </c>
       <c r="G6" s="3"/>
@@ -746,34 +1211,36 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3">
-        <f t="shared" ref="L6:L7" si="5">H6+I6+J6+K6</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="3" t="e">
-        <f t="shared" ref="M6:M7" si="6">((H6+I6)/(H6+I6+J6+K6))*100</f>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="3" t="e">
+        <f t="shared" ref="O6:O7" si="4">((J6+K6)/(J6+K6+L6+M6))*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="3" t="e">
-        <f t="shared" ref="N6:N7" si="7">(H6/(H6+I6))*100</f>
+      <c r="P6" s="3" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G7" s="3"/>
@@ -781,32 +1248,35 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="3" t="e">
-        <f t="shared" si="6"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="3" t="e">
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N7" s="3" t="e">
-        <f t="shared" si="7"/>
+      <c r="P7" s="3" t="e">
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
+  <mergeCells count="10">
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:R1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
5th testing of OB using 1419 data, 5 epoch, and do the spliting data to data train & test
</commit_message>
<xml_diff>
--- a/result/result training.xlsx
+++ b/result/result training.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\number-plate-recognition\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5CA58D-69AF-46D9-A481-20B740552B9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34EF03B-A8AA-4AE1-BBF7-94DDA40C9A42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Real" sheetId="3" r:id="rId1"/>
-    <sheet name="Modif" sheetId="5" r:id="rId2"/>
+    <sheet name="Before" sheetId="6" r:id="rId2"/>
+    <sheet name="Modif" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
   <si>
     <t>Train</t>
   </si>
@@ -101,6 +102,12 @@
   </si>
   <si>
     <t>runs\detect\train212</t>
+  </si>
+  <si>
+    <t>runs\detect\train22</t>
+  </si>
+  <si>
+    <t>runs\detect\train222</t>
   </si>
 </sst>
 </file>
@@ -228,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -255,14 +262,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -273,11 +286,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,71 +507,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BF86F8-5004-4712-B9DC-99E03C733B38}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="1" customWidth="1"/>
-    <col min="10" max="14" width="9.109375" style="1"/>
-    <col min="15" max="15" width="11" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.109375" style="1" customWidth="1"/>
-    <col min="17" max="18" width="21.6640625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="11" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="21.7109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="10" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="H1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10" t="s">
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="N1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="O1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="15"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="17"/>
+      <c r="P1" s="17"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
@@ -571,38 +578,32 @@
       <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="8" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="P2" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -624,6 +625,511 @@
         <v>44</v>
       </c>
       <c r="G3" s="3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>44</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f>H3+I3+J3+K3</f>
+        <v>44</v>
+      </c>
+      <c r="M3" s="3">
+        <f>((H3+I3)/(H3+I3+J3+K3))*100</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="3" t="e">
+        <f>(H3/(H3+I3))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>817</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D4" s="3">
+        <f>ROUNDUP(C4*B4,0)</f>
+        <v>736</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="3">
+        <f>ROUNDDOWN(E4*B4,0)</f>
+        <v>81</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3">
+        <v>45</v>
+      </c>
+      <c r="I4" s="3">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3">
+        <v>36</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L5" si="0">H4+I4+J4+K4</f>
+        <v>101</v>
+      </c>
+      <c r="M4" s="5">
+        <f>((H4+I4)/(H4+I4+J4+K4))*100</f>
+        <v>64.356435643564353</v>
+      </c>
+      <c r="N4" s="5">
+        <f t="shared" ref="N4:N5" si="1">(H4/(H4+I4))*100</f>
+        <v>69.230769230769226</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>817</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D5" s="3">
+        <f>ROUNDUP(C5*B5,0)</f>
+        <v>736</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="3">
+        <f>ROUNDDOWN(E5*B5,0)</f>
+        <v>81</v>
+      </c>
+      <c r="G5" s="3">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3">
+        <v>77</v>
+      </c>
+      <c r="I5" s="3">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3">
+        <v>4</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="M5" s="5">
+        <f>((H5+I5)/(H5+I5+J5+K5))*100</f>
+        <v>95.604395604395606</v>
+      </c>
+      <c r="N5" s="5">
+        <f t="shared" si="1"/>
+        <v>88.505747126436788</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1277</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1135</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>142</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>120</v>
+      </c>
+      <c r="I6" s="3">
+        <v>24</v>
+      </c>
+      <c r="J6" s="3">
+        <v>22</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" ref="L6:L7" si="2">H6+I6+J6+K6</f>
+        <v>166</v>
+      </c>
+      <c r="M6" s="5">
+        <f t="shared" ref="M6:M7" si="3">((H6+I6)/(H6+I6+J6+K6))*100</f>
+        <v>86.746987951807228</v>
+      </c>
+      <c r="N6" s="5">
+        <f t="shared" ref="N6:N7" si="4">(H6/(H6+I6))*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1419</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D7" s="3">
+        <f>ROUND(C7*B7,0)</f>
+        <v>1277</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="3">
+        <f>ROUND(E7*B7,0)</f>
+        <v>142</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>123</v>
+      </c>
+      <c r="I7" s="3">
+        <v>61</v>
+      </c>
+      <c r="J7" s="3">
+        <v>22</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="2"/>
+        <v>206</v>
+      </c>
+      <c r="M7" s="5">
+        <f t="shared" si="3"/>
+        <v>89.320388349514573</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="4"/>
+        <v>66.847826086956516</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1419</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ref="D8:D10" si="5">ROUND(C8*B8,0)</f>
+        <v>1277</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" ref="F8:F10" si="6">ROUND(E8*B8,0)</f>
+        <v>142</v>
+      </c>
+      <c r="G8" s="3">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3">
+        <f t="shared" ref="L8:L10" si="7">H8+I8+J8+K8</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="5" t="e">
+        <f t="shared" ref="M8:M10" si="8">((H8+I8)/(H8+I8+J8+K8))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="5" t="e">
+        <f t="shared" ref="N8:N10" si="9">(H8/(H8+I8))*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="5" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="5" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA65D9D-BF3A-4FF3-9498-C94214E8AE6D}">
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
+    <col min="10" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="11" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="1" customWidth="1"/>
+    <col min="17" max="18" width="21.7109375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="17"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>440</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D3" s="3">
+        <f>ROUNDUP(C3*B3,0)</f>
+        <v>396</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="3">
+        <f>ROUNDDOWN(E3*B3,0)</f>
+        <v>44</v>
+      </c>
+      <c r="G3" s="3">
         <v>0</v>
       </c>
       <c r="H3" s="3">
@@ -660,7 +1166,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -685,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H7" si="0">G4*B4</f>
+        <f t="shared" ref="H4:H5" si="0">G4*B4</f>
         <v>0</v>
       </c>
       <c r="I4" s="3">
@@ -704,7 +1210,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" ref="N4:N5" si="1">J4+K4+L4+M4</f>
+        <f t="shared" ref="N4:N7" si="1">J4+K4+L4+M4</f>
         <v>101</v>
       </c>
       <c r="O4" s="5">
@@ -712,7 +1218,7 @@
         <v>64.356435643564353</v>
       </c>
       <c r="P4" s="5">
-        <f t="shared" ref="P4:P5" si="2">(J4/(J4+K4))*100</f>
+        <f t="shared" ref="P4:P7" si="2">(J4/(J4+K4))*100</f>
         <v>69.230769230769226</v>
       </c>
       <c r="Q4" s="3" t="s">
@@ -722,7 +1228,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -784,7 +1290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -828,15 +1334,15 @@
         <v>0</v>
       </c>
       <c r="N6" s="3">
-        <f t="shared" ref="N6:N7" si="3">J6+K6+L6+M6</f>
+        <f t="shared" si="1"/>
         <v>166</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" ref="O6:O7" si="4">((J6+K6)/(J6+K6+L6+M6))*100</f>
+        <f t="shared" ref="O6:O7" si="3">((J6+K6)/(J6+K6+L6+M6))*100</f>
         <v>86.746987951807228</v>
       </c>
       <c r="P6" s="5">
-        <f t="shared" ref="P6:P7" si="5">(J6/(J6+K6))*100</f>
+        <f t="shared" si="2"/>
         <v>83.333333333333343</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -846,7 +1352,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -872,15 +1378,15 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="3" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="3" t="e">
-        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P7" s="3" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q7" s="3"/>
@@ -888,15 +1394,15 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:R1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C1:D1"/>
     <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -904,7 +1410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5ED25B5-2FA0-42FF-A500-B0ACF9209455}">
   <dimension ref="A1:R7"/>
   <sheetViews>
@@ -912,65 +1418,65 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" customWidth="1"/>
-    <col min="10" max="14" width="9.109375" style="1"/>
+    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" customWidth="1"/>
+    <col min="10" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="11" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.109375" style="1" customWidth="1"/>
-    <col min="17" max="18" width="21.6640625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="1"/>
+    <col min="16" max="16" width="14.140625" style="1" customWidth="1"/>
+    <col min="17" max="18" width="21.7109375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="13" t="s">
+      <c r="F1" s="16"/>
+      <c r="G1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="10" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="15"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="R1" s="17"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
@@ -989,7 +1495,7 @@
       <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="11"/>
+      <c r="I2" s="12"/>
       <c r="J2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1005,8 +1511,8 @@
       <c r="N2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="19"/>
       <c r="Q2" s="8" t="s">
         <v>16</v>
       </c>
@@ -1014,7 +1520,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1071,7 +1577,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1131,7 +1637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1191,7 +1697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1203,7 +1709,7 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3">
-        <f t="shared" ref="F4:F7" si="3">B6-D6</f>
+        <f t="shared" ref="F6:F7" si="3">B6-D6</f>
         <v>0</v>
       </c>
       <c r="G6" s="3"/>
@@ -1228,7 +1734,7 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
6th testing of OB using 1419 data, 10 epoch, and do the spliting data to data train & test
</commit_message>
<xml_diff>
--- a/result/result training.xlsx
+++ b/result/result training.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\number-plate-recognition\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34EF03B-A8AA-4AE1-BBF7-94DDA40C9A42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7E93DA-28DD-49ED-AB40-E0A3620C1E0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1428" yWindow="720" windowWidth="21600" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Real" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="28">
   <si>
     <t>Train</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>runs\detect\train222</t>
+  </si>
+  <si>
+    <t>runs\detect\train23</t>
+  </si>
+  <si>
+    <t>runs\detect\train232</t>
   </si>
 </sst>
 </file>
@@ -510,24 +516,24 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
-    <col min="8" max="12" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
+    <col min="8" max="12" width="9.109375" style="1"/>
     <col min="13" max="13" width="11" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="21.7109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="14" width="14.109375" style="1" customWidth="1"/>
+    <col min="15" max="16" width="21.6640625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
@@ -563,7 +569,7 @@
       </c>
       <c r="P1" s="17"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="14"/>
       <c r="C2" s="2" t="s">
@@ -603,7 +609,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -654,7 +660,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -709,7 +715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -764,7 +770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -817,7 +823,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -872,7 +878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -896,26 +902,38 @@
       <c r="G8" s="3">
         <v>10</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="H8" s="3">
+        <v>123</v>
+      </c>
+      <c r="I8" s="3">
+        <v>8</v>
+      </c>
+      <c r="J8" s="3">
+        <v>22</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
       <c r="L8" s="3">
         <f t="shared" ref="L8:L10" si="7">H8+I8+J8+K8</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="5" t="e">
+        <v>153</v>
+      </c>
+      <c r="M8" s="5">
         <f t="shared" ref="M8:M10" si="8">((H8+I8)/(H8+I8+J8+K8))*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N8" s="5" t="e">
+        <v>85.620915032679733</v>
+      </c>
+      <c r="N8" s="5">
         <f t="shared" ref="N8:N10" si="9">(H8/(H8+I8))*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>93.893129770992374</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -948,7 +966,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1006,23 +1024,23 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
-    <col min="10" max="14" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
+    <col min="10" max="14" width="9.109375" style="1"/>
     <col min="15" max="15" width="11" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" customWidth="1"/>
-    <col min="17" max="18" width="21.7109375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16" width="14.109375" style="1" customWidth="1"/>
+    <col min="17" max="18" width="21.6640625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
@@ -1062,7 +1080,7 @@
       </c>
       <c r="R1" s="17"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="14"/>
       <c r="C2" s="9" t="s">
@@ -1108,7 +1126,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1166,7 +1184,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1228,7 +1246,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1290,7 +1308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1352,7 +1370,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1418,23 +1436,23 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="1" customWidth="1"/>
-    <col min="10" max="14" width="9.140625" style="1"/>
+    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="1" customWidth="1"/>
+    <col min="10" max="14" width="9.109375" style="1"/>
     <col min="15" max="15" width="11" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="1" customWidth="1"/>
-    <col min="17" max="18" width="21.7109375" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16" width="14.109375" style="1" customWidth="1"/>
+    <col min="17" max="18" width="21.6640625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
@@ -1474,7 +1492,7 @@
       </c>
       <c r="R1" s="17"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="6" t="s">
@@ -1520,7 +1538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1577,7 +1595,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1637,7 +1655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1697,7 +1715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1734,7 +1752,7 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
7th testing of OB using 1776 data, 5 epoch, and do the spliting data to data train & test
</commit_message>
<xml_diff>
--- a/result/result training.xlsx
+++ b/result/result training.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\number-plate-recognition\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7E93DA-28DD-49ED-AB40-E0A3620C1E0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B9F727-C608-42BD-B63F-77697F4C0D69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="720" windowWidth="21600" windowHeight="11832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Real" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
   <si>
     <t>Train</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>runs\detect\train232</t>
+  </si>
+  <si>
+    <t>runs\detect\train24</t>
+  </si>
+  <si>
+    <t>runs\detect\train242</t>
   </si>
 </sst>
 </file>
@@ -137,7 +143,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +153,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -241,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -269,6 +281,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -516,7 +534,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -534,44 +552,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="11" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="11" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="17"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="14"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
@@ -584,7 +602,7 @@
       <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
@@ -600,8 +618,8 @@
       <c r="L2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="19"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="21"/>
       <c r="O2" s="8" t="s">
         <v>16</v>
       </c>
@@ -771,55 +789,55 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="11">
         <v>1277</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="11">
         <v>0.9</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="11">
         <v>1135</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="11">
         <v>0.1</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="11">
         <v>142</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="11">
         <v>5</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="11">
         <v>120</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="11">
         <v>24</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="11">
         <v>22</v>
       </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3">
+      <c r="K6" s="11">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11">
         <f t="shared" ref="L6:L7" si="2">H6+I6+J6+K6</f>
         <v>166</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="12">
         <f t="shared" ref="M6:M7" si="3">((H6+I6)/(H6+I6+J6+K6))*100</f>
         <v>86.746987951807228</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="12">
         <f t="shared" ref="N6:N7" si="4">(H6/(H6+I6))*100</f>
         <v>83.333333333333343</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="11" t="s">
         <v>23</v>
       </c>
     </row>
@@ -934,40 +952,64 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1776</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.9</v>
+      </c>
       <c r="D9" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>1598</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.1</v>
+      </c>
       <c r="F9" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+        <v>178</v>
+      </c>
+      <c r="G9" s="3">
+        <v>5</v>
+      </c>
+      <c r="H9" s="3">
+        <v>156</v>
+      </c>
+      <c r="I9" s="3">
+        <v>73</v>
+      </c>
+      <c r="J9" s="3">
+        <v>25</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
       <c r="L9" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="5" t="e">
+        <v>254</v>
+      </c>
+      <c r="M9" s="5">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N9" s="5" t="e">
+        <v>90.157480314960623</v>
+      </c>
+      <c r="N9" s="5">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+        <v>68.122270742358083</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
@@ -1041,48 +1083,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="11" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="11" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="Q1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="17"/>
+      <c r="R1" s="19"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="14"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
@@ -1101,7 +1143,7 @@
       <c r="H2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="12"/>
+      <c r="I2" s="14"/>
       <c r="J2" s="10" t="s">
         <v>3</v>
       </c>
@@ -1117,8 +1159,8 @@
       <c r="N2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="19"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="21"/>
       <c r="Q2" s="8" t="s">
         <v>16</v>
       </c>
@@ -1453,48 +1495,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="11" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="11" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="Q1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="17"/>
+      <c r="R1" s="19"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1513,7 +1555,7 @@
       <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="12"/>
+      <c r="I2" s="14"/>
       <c r="J2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1529,8 +1571,8 @@
       <c r="N2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="19"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="21"/>
       <c r="Q2" s="8" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
8th testing of OB using 1776 data, 10 epoch, and do the spliting data to data train & test. Then create presentation
</commit_message>
<xml_diff>
--- a/result/result training.xlsx
+++ b/result/result training.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\number-plate-recognition\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B9F727-C608-42BD-B63F-77697F4C0D69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B937D86A-216D-49BC-BD81-89D17514A893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
   <si>
     <t>Train</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>runs\detect\train242</t>
+  </si>
+  <si>
+    <t>runs\detect\train25</t>
+  </si>
+  <si>
+    <t>runs\detect\train252</t>
   </si>
 </sst>
 </file>
@@ -253,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -286,7 +292,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -534,62 +543,62 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
-    <col min="8" max="12" width="9.109375" style="1"/>
+    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="11" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" style="1" customWidth="1"/>
-    <col min="15" max="16" width="21.6640625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="14" max="14" width="14.140625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="21.7109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="17" t="s">
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="13" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="13" t="s">
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="19"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="16"/>
+      <c r="P1" s="20"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
@@ -602,7 +611,7 @@
       <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="15"/>
       <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
@@ -618,8 +627,8 @@
       <c r="L2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="21"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="22"/>
       <c r="O2" s="8" t="s">
         <v>16</v>
       </c>
@@ -627,7 +636,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -678,7 +687,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -718,11 +727,11 @@
         <f t="shared" ref="L4:L5" si="0">H4+I4+J4+K4</f>
         <v>101</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="12">
         <f>((H4+I4)/(H4+I4+J4+K4))*100</f>
         <v>64.356435643564353</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="12">
         <f t="shared" ref="N4:N5" si="1">(H4/(H4+I4))*100</f>
         <v>69.230769230769226</v>
       </c>
@@ -733,7 +742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -773,11 +782,11 @@
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="12">
         <f>((H5+I5)/(H5+I5+J5+K5))*100</f>
         <v>95.604395604395606</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="12">
         <f t="shared" si="1"/>
         <v>88.505747126436788</v>
       </c>
@@ -788,7 +797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -826,11 +835,11 @@
         <f t="shared" ref="L6:L7" si="2">H6+I6+J6+K6</f>
         <v>166</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="13">
         <f t="shared" ref="M6:M7" si="3">((H6+I6)/(H6+I6+J6+K6))*100</f>
         <v>86.746987951807228</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="13">
         <f t="shared" ref="N6:N7" si="4">(H6/(H6+I6))*100</f>
         <v>83.333333333333343</v>
       </c>
@@ -841,7 +850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -881,11 +890,11 @@
         <f t="shared" si="2"/>
         <v>206</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="12">
         <f t="shared" si="3"/>
         <v>89.320388349514573</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="12">
         <f t="shared" si="4"/>
         <v>66.847826086956516</v>
       </c>
@@ -896,7 +905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -936,11 +945,11 @@
         <f t="shared" ref="L8:L10" si="7">H8+I8+J8+K8</f>
         <v>153</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="12">
         <f t="shared" ref="M8:M10" si="8">((H8+I8)/(H8+I8+J8+K8))*100</f>
         <v>85.620915032679733</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="12">
         <f t="shared" ref="N8:N10" si="9">(H8/(H8+I8))*100</f>
         <v>93.893129770992374</v>
       </c>
@@ -951,7 +960,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -991,11 +1000,11 @@
         <f t="shared" si="7"/>
         <v>254</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="12">
         <f t="shared" si="8"/>
         <v>90.157480314960623</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="12">
         <f t="shared" si="9"/>
         <v>68.122270742358083</v>
       </c>
@@ -1006,40 +1015,60 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="3">
+        <v>1776</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.9</v>
+      </c>
       <c r="D10" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>1598</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.1</v>
+      </c>
       <c r="F10" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+        <v>178</v>
+      </c>
+      <c r="G10" s="3">
+        <v>10</v>
+      </c>
+      <c r="H10" s="3">
+        <v>163</v>
+      </c>
+      <c r="I10" s="3">
+        <v>30</v>
+      </c>
+      <c r="J10" s="3">
+        <v>18</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
       <c r="L10" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="5" t="e">
+        <v>211</v>
+      </c>
+      <c r="M10" s="12">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N10" s="5" t="e">
+        <v>91.469194312796205</v>
+      </c>
+      <c r="N10" s="12">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+        <v>84.4559585492228</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1066,65 +1095,65 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
-    <col min="10" max="14" width="9.109375" style="1"/>
+    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
+    <col min="10" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="11" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.109375" style="1" customWidth="1"/>
-    <col min="17" max="18" width="21.6640625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="1"/>
+    <col min="16" max="16" width="14.140625" style="1" customWidth="1"/>
+    <col min="17" max="18" width="21.7109375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="17" t="s">
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="13" t="s">
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="19"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="16"/>
+      <c r="R1" s="20"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
@@ -1143,7 +1172,7 @@
       <c r="H2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="14"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="10" t="s">
         <v>3</v>
       </c>
@@ -1159,8 +1188,8 @@
       <c r="N2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="21"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="22"/>
       <c r="Q2" s="8" t="s">
         <v>16</v>
       </c>
@@ -1168,7 +1197,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1226,7 +1255,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1288,7 +1317,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1350,7 +1379,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1412,7 +1441,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1478,65 +1507,65 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" customWidth="1"/>
-    <col min="10" max="14" width="9.109375" style="1"/>
+    <col min="3" max="5" width="10.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" customWidth="1"/>
+    <col min="10" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="11" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.109375" style="1" customWidth="1"/>
-    <col min="17" max="18" width="21.6640625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="1"/>
+    <col min="16" max="16" width="14.140625" style="1" customWidth="1"/>
+    <col min="17" max="18" width="21.7109375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="17" t="s">
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="19"/>
+      <c r="E1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="13" t="s">
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="19"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
+      <c r="R1" s="20"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1555,7 +1584,7 @@
       <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="14"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1571,8 +1600,8 @@
       <c r="N2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="21"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="22"/>
       <c r="Q2" s="8" t="s">
         <v>16</v>
       </c>
@@ -1580,7 +1609,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1637,7 +1666,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1697,7 +1726,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1757,7 +1786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1794,7 +1823,7 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
create function for training model
</commit_message>
<xml_diff>
--- a/result/result training.xlsx
+++ b/result/result training.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\number-plate-recognition\result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\New folder\number-plate-recognition\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B937D86A-216D-49BC-BD81-89D17514A893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A4A7E3-8872-41EC-9556-4CBACDAF98DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Real" sheetId="3" r:id="rId1"/>
@@ -149,7 +149,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +165,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -323,6 +329,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -543,7 +555,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -946,7 +958,7 @@
         <v>153</v>
       </c>
       <c r="M8" s="12">
-        <f t="shared" ref="M8:M10" si="8">((H8+I8)/(H8+I8+J8+K8))*100</f>
+        <f t="shared" ref="M8:M9" si="8">((H8+I8)/(H8+I8+J8+K8))*100</f>
         <v>85.620915032679733</v>
       </c>
       <c r="N8" s="12">
@@ -1016,57 +1028,57 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="23">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="23">
         <v>1776</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="23">
         <v>0.9</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="23">
         <f t="shared" si="5"/>
         <v>1598</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="23">
         <v>0.1</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="23">
         <f t="shared" si="6"/>
         <v>178</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="23">
         <v>10</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="23">
         <v>163</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="23">
         <v>30</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="23">
         <v>18</v>
       </c>
-      <c r="K10" s="3">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3">
+      <c r="K10" s="23">
+        <v>0</v>
+      </c>
+      <c r="L10" s="23">
         <f t="shared" si="7"/>
         <v>211</v>
       </c>
-      <c r="M10" s="12">
-        <f t="shared" si="8"/>
+      <c r="M10" s="24">
+        <f>((H10+I10)/(H10+I10+J10+K10))*100</f>
         <v>91.469194312796205</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="24">
         <f t="shared" si="9"/>
         <v>84.4559585492228</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="O10" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" s="23" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>